<commit_message>
new input for exp
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/for paper/input with changes.xlsx
+++ b/migforecasting/clustering/for paper/input with changes.xlsx
@@ -520,13 +520,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>5648.558240191881</v>
+        <v>3074.994130329068</v>
       </c>
       <c r="C2" t="n">
         <v>20815.4167831292</v>
       </c>
       <c r="D2" t="n">
-        <v>19721.96170086985</v>
+        <v>9990.927465433009</v>
       </c>
       <c r="E2" t="n">
         <v>881.0076688693483</v>
@@ -538,22 +538,22 @@
         <v>39.4</v>
       </c>
       <c r="H2" t="n">
-        <v>125.6772308691166</v>
+        <v>52.28189156677908</v>
       </c>
       <c r="I2" t="n">
-        <v>77.80585983126005</v>
+        <v>9.829484154314454</v>
       </c>
       <c r="J2" t="n">
-        <v>657.7753259148542</v>
+        <v>338.9834683803142</v>
       </c>
       <c r="K2" t="n">
-        <v>101102.9756497258</v>
+        <v>35709.00890922388</v>
       </c>
       <c r="L2" t="n">
-        <v>120574.1931586198</v>
+        <v>73632.72488415125</v>
       </c>
       <c r="M2" t="n">
-        <v>4717355.206267274</v>
+        <v>744853.9651349846</v>
       </c>
       <c r="N2" t="n">
         <v>35.75225116085909</v>
@@ -562,7 +562,7 @@
         <v>1599.139320430128</v>
       </c>
       <c r="P2" t="n">
-        <v>5013077.512856801</v>
+        <v>356159.9599555623</v>
       </c>
     </row>
     <row r="3">
@@ -650,10 +650,10 @@
         <v>208310</v>
       </c>
       <c r="L4" t="n">
-        <v>120574.1931586198</v>
+        <v>73217.65388798401</v>
       </c>
       <c r="M4" t="n">
-        <v>4717355.206267274</v>
+        <v>2545166.61841985</v>
       </c>
       <c r="N4" t="n">
         <v>40.99999999999991</v>
@@ -676,13 +676,13 @@
         <v>21712.38264</v>
       </c>
       <c r="D5" t="n">
-        <v>19721.96170086985</v>
+        <v>10065.87483001023</v>
       </c>
       <c r="E5" t="n">
         <v>881.0076688693483</v>
       </c>
       <c r="F5" t="n">
-        <v>1094086.860592877</v>
+        <v>693877.7992514279</v>
       </c>
       <c r="G5" t="n">
         <v>38.2</v>
@@ -697,10 +697,10 @@
         <v>657.7753259148542</v>
       </c>
       <c r="K5" t="n">
-        <v>101102.9756497258</v>
+        <v>16451.42835168915</v>
       </c>
       <c r="L5" t="n">
-        <v>120574.1931586198</v>
+        <v>44614.97432854872</v>
       </c>
       <c r="M5" t="n">
         <v>4968189.53784</v>
@@ -712,7 +712,7 @@
         <v>1599.139320430128</v>
       </c>
       <c r="P5" t="n">
-        <v>5013077.512856801</v>
+        <v>2603925.131103361</v>
       </c>
     </row>
     <row r="6">
@@ -750,7 +750,7 @@
         <v>127583</v>
       </c>
       <c r="L6" t="n">
-        <v>120574.1931586198</v>
+        <v>69713.06049263012</v>
       </c>
       <c r="M6" t="n">
         <v>5517088.419299998</v>
@@ -797,16 +797,16 @@
         <v>384.7889277610419</v>
       </c>
       <c r="K7" t="n">
-        <v>28977.99857868786</v>
+        <v>10711.99999999995</v>
       </c>
       <c r="L7" t="n">
-        <v>24766.25131576219</v>
+        <v>8164.16900863609</v>
       </c>
       <c r="M7" t="n">
-        <v>827690.0633385038</v>
+        <v>54366.53152584554</v>
       </c>
       <c r="N7" t="n">
-        <v>21.09561578308453</v>
+        <v>1.999999999999993</v>
       </c>
       <c r="O7" t="n">
         <v>2896.85900668096</v>
@@ -847,13 +847,13 @@
         <v>962.7999999999989</v>
       </c>
       <c r="K8" t="n">
-        <v>28977.99857868786</v>
+        <v>8125.999999999992</v>
       </c>
       <c r="L8" t="n">
         <v>44861.88999999995</v>
       </c>
       <c r="M8" t="n">
-        <v>827690.0633385038</v>
+        <v>216908.5926211885</v>
       </c>
       <c r="N8" t="n">
         <v>33.99999999999992</v>
@@ -870,16 +870,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>10206.30689960662</v>
+        <v>4564.627890295273</v>
       </c>
       <c r="C9" t="n">
         <v>37917.46208</v>
       </c>
       <c r="D9" t="n">
-        <v>45468.34750546934</v>
+        <v>16177.06409222068</v>
       </c>
       <c r="E9" t="n">
-        <v>1645.641044300649</v>
+        <v>737.7220073590736</v>
       </c>
       <c r="F9" t="n">
         <v>2362294.764186412</v>
@@ -897,10 +897,10 @@
         <v>384.7889277610419</v>
       </c>
       <c r="K9" t="n">
-        <v>28977.99857868786</v>
+        <v>4886.999999999982</v>
       </c>
       <c r="L9" t="n">
-        <v>24766.25131576219</v>
+        <v>9316.235897955692</v>
       </c>
       <c r="M9" t="n">
         <v>827690.0633385038</v>
@@ -909,7 +909,7 @@
         <v>21.09561578308453</v>
       </c>
       <c r="O9" t="n">
-        <v>2896.85900668096</v>
+        <v>1143.729881414369</v>
       </c>
       <c r="P9" t="n">
         <v>8379778.190979367</v>
@@ -947,16 +947,16 @@
         <v>384.7889277610419</v>
       </c>
       <c r="K10" t="n">
-        <v>28977.99857868786</v>
+        <v>2243.999999999904</v>
       </c>
       <c r="L10" t="n">
-        <v>24766.25131576219</v>
+        <v>13298.13054705717</v>
       </c>
       <c r="M10" t="n">
-        <v>827690.0633385038</v>
+        <v>184575.0998610461</v>
       </c>
       <c r="N10" t="n">
-        <v>21.09561578308453</v>
+        <v>5.999999999999972</v>
       </c>
       <c r="O10" t="n">
         <v>3302</v>
@@ -1026,13 +1026,13 @@
         <v>19210.2288312461</v>
       </c>
       <c r="D12" t="n">
-        <v>7762.675320911603</v>
+        <v>3746.599999999997</v>
       </c>
       <c r="E12" t="n">
-        <v>281.9402175474014</v>
+        <v>44.99999999999995</v>
       </c>
       <c r="F12" t="n">
-        <v>374829.3789556442</v>
+        <v>84821.61661287429</v>
       </c>
       <c r="G12" t="n">
         <v>35.4380373831775</v>
@@ -1041,10 +1041,10 @@
         <v>54.0725142426617</v>
       </c>
       <c r="I12" t="n">
-        <v>28.22123465014427</v>
+        <v>9.999999999999948</v>
       </c>
       <c r="J12" t="n">
-        <v>479.1465622563072</v>
+        <v>220.5462165225156</v>
       </c>
       <c r="K12" t="n">
         <v>32749.97834610207</v>
@@ -1053,7 +1053,7 @@
         <v>14259.05628514748</v>
       </c>
       <c r="M12" t="n">
-        <v>1321756.113011211</v>
+        <v>633508.489027101</v>
       </c>
       <c r="N12" t="n">
         <v>22.70687713300876</v>
@@ -1062,7 +1062,7 @@
         <v>672.9999999999999</v>
       </c>
       <c r="P12" t="n">
-        <v>1212990.425859435</v>
+        <v>286032.9961373269</v>
       </c>
     </row>
     <row r="13">
@@ -1179,10 +1179,10 @@
         <v>7762.675320911603</v>
       </c>
       <c r="E15" t="n">
-        <v>281.9402175474014</v>
+        <v>130.9999999999998</v>
       </c>
       <c r="F15" t="n">
-        <v>374829.3789556442</v>
+        <v>153719.0900088869</v>
       </c>
       <c r="G15" t="n">
         <v>35.4380373831775</v>
@@ -1191,7 +1191,7 @@
         <v>103.9999999999993</v>
       </c>
       <c r="I15" t="n">
-        <v>28.22123465014427</v>
+        <v>2.999999999999976</v>
       </c>
       <c r="J15" t="n">
         <v>479.1465622563072</v>
@@ -1270,49 +1270,49 @@
         <v>3</v>
       </c>
       <c r="B17" t="n">
-        <v>5714.508054533066</v>
+        <v>1056.473753859249</v>
       </c>
       <c r="C17" t="n">
         <v>20427.3418483414</v>
       </c>
       <c r="D17" t="n">
-        <v>18620.07860285665</v>
+        <v>2381.065679515827</v>
       </c>
       <c r="E17" t="n">
-        <v>713.9226602467268</v>
+        <v>113.4249949517034</v>
       </c>
       <c r="F17" t="n">
-        <v>795019.6038440204</v>
+        <v>81501.24624526063</v>
       </c>
       <c r="G17" t="n">
         <v>35.8</v>
       </c>
       <c r="H17" t="n">
-        <v>121.2195445843775</v>
+        <v>15.9825267133037</v>
       </c>
       <c r="I17" t="n">
-        <v>82.574144705994</v>
+        <v>2.573634099879445</v>
       </c>
       <c r="J17" t="n">
-        <v>675.1104937785783</v>
+        <v>109.9937054332045</v>
       </c>
       <c r="K17" t="n">
-        <v>390629.3741131953</v>
+        <v>44335.91368807349</v>
       </c>
       <c r="L17" t="n">
-        <v>50169.9141912</v>
+        <v>2003.262820579908</v>
       </c>
       <c r="M17" t="n">
-        <v>5170690.3577638</v>
+        <v>1077875.228372509</v>
       </c>
       <c r="N17" t="n">
-        <v>37.03779183275061</v>
+        <v>11.57791462094847</v>
       </c>
       <c r="O17" t="n">
-        <v>1578.038753022092</v>
+        <v>315.8466231128759</v>
       </c>
       <c r="P17" t="n">
-        <v>5162046.502920203</v>
+        <v>1122077.832194185</v>
       </c>
     </row>
     <row r="18">
@@ -1329,10 +1329,10 @@
         <v>18620.07860285665</v>
       </c>
       <c r="E18" t="n">
-        <v>713.9226602467268</v>
+        <v>39.69874823309618</v>
       </c>
       <c r="F18" t="n">
-        <v>795019.6038440204</v>
+        <v>377439.3726886988</v>
       </c>
       <c r="G18" t="n">
         <v>28.8591707317073</v>
@@ -1344,13 +1344,13 @@
         <v>82.574144705994</v>
       </c>
       <c r="J18" t="n">
-        <v>675.1104937785783</v>
+        <v>273.7681169627428</v>
       </c>
       <c r="K18" t="n">
         <v>390629.3741131953</v>
       </c>
       <c r="L18" t="n">
-        <v>50169.9141912</v>
+        <v>30552.937259517</v>
       </c>
       <c r="M18" t="n">
         <v>5170690.3577638</v>
@@ -1370,19 +1370,19 @@
         <v>3</v>
       </c>
       <c r="B19" t="n">
-        <v>5714.508054533066</v>
+        <v>2528.038589716432</v>
       </c>
       <c r="C19" t="n">
         <v>20427.3418483414</v>
       </c>
       <c r="D19" t="n">
-        <v>18620.07860285665</v>
+        <v>11096.21063674203</v>
       </c>
       <c r="E19" t="n">
-        <v>713.9226602467268</v>
+        <v>333.1859226706291</v>
       </c>
       <c r="F19" t="n">
-        <v>795019.6038440204</v>
+        <v>480263.6654099055</v>
       </c>
       <c r="G19" t="n">
         <v>28.8591707317073</v>
@@ -1397,13 +1397,13 @@
         <v>675.1104937785783</v>
       </c>
       <c r="K19" t="n">
-        <v>390629.3741131953</v>
+        <v>253392.3988960179</v>
       </c>
       <c r="L19" t="n">
-        <v>50169.9141912</v>
+        <v>30747.73245897568</v>
       </c>
       <c r="M19" t="n">
-        <v>5170690.3577638</v>
+        <v>3041350.614883801</v>
       </c>
       <c r="N19" t="n">
         <v>37.03779183275061</v>
@@ -1412,7 +1412,7 @@
         <v>1578.038753022092</v>
       </c>
       <c r="P19" t="n">
-        <v>5162046.502920203</v>
+        <v>482329.4836359872</v>
       </c>
     </row>
     <row r="20">
@@ -1453,7 +1453,7 @@
         <v>104307.93</v>
       </c>
       <c r="M20" t="n">
-        <v>5170690.3577638</v>
+        <v>2846566.710468096</v>
       </c>
       <c r="N20" t="n">
         <v>37.03779183275061</v>
@@ -1544,19 +1544,19 @@
         <v>171.9999999999993</v>
       </c>
       <c r="J22" t="n">
-        <v>515.0943407417118</v>
+        <v>201.0999999999998</v>
       </c>
       <c r="K22" t="n">
-        <v>49395.30627568397</v>
+        <v>14598.99999999995</v>
       </c>
       <c r="L22" t="n">
-        <v>37819.7689054316</v>
+        <v>23998.86785081873</v>
       </c>
       <c r="M22" t="n">
-        <v>1725327.064726412</v>
+        <v>286065.1040134371</v>
       </c>
       <c r="N22" t="n">
-        <v>25.90492510159179</v>
+        <v>10.99999999999997</v>
       </c>
       <c r="O22" t="n">
         <v>2915.76176821649</v>
@@ -1576,13 +1576,13 @@
         <v>34591.61742</v>
       </c>
       <c r="D23" t="n">
-        <v>38299.68163489593</v>
+        <v>16196.06113338833</v>
       </c>
       <c r="E23" t="n">
-        <v>1288.588016602401</v>
+        <v>593.7048669751483</v>
       </c>
       <c r="F23" t="n">
-        <v>2114276.549986417</v>
+        <v>198628.8662816901</v>
       </c>
       <c r="G23" t="n">
         <v>27.9654227272727</v>
@@ -1594,19 +1594,19 @@
         <v>132.0329562209512</v>
       </c>
       <c r="J23" t="n">
-        <v>515.0943407417118</v>
+        <v>169.2999999999999</v>
       </c>
       <c r="K23" t="n">
-        <v>49395.30627568397</v>
+        <v>19625.99999999998</v>
       </c>
       <c r="L23" t="n">
-        <v>37819.7689054316</v>
+        <v>14867.20570471301</v>
       </c>
       <c r="M23" t="n">
-        <v>1725327.064726412</v>
+        <v>527779.8131531713</v>
       </c>
       <c r="N23" t="n">
-        <v>25.90492510159179</v>
+        <v>11.99999999999997</v>
       </c>
       <c r="O23" t="n">
         <v>2915.76176821649</v>
@@ -1644,19 +1644,19 @@
         <v>232.999999999999</v>
       </c>
       <c r="J24" t="n">
-        <v>515.0943407417118</v>
+        <v>188.4999999999993</v>
       </c>
       <c r="K24" t="n">
-        <v>49395.30627568397</v>
+        <v>1592.999999999883</v>
       </c>
       <c r="L24" t="n">
         <v>37819.7689054316</v>
       </c>
       <c r="M24" t="n">
-        <v>1725327.064726412</v>
+        <v>385565.2847686771</v>
       </c>
       <c r="N24" t="n">
-        <v>25.90492510159179</v>
+        <v>7.999999999999967</v>
       </c>
       <c r="O24" t="n">
         <v>5536</v>
@@ -1694,19 +1694,19 @@
         <v>230.999999999999</v>
       </c>
       <c r="J25" t="n">
-        <v>515.0943407417118</v>
+        <v>233.2999999999996</v>
       </c>
       <c r="K25" t="n">
-        <v>49395.30627568397</v>
+        <v>383.99999999993</v>
       </c>
       <c r="L25" t="n">
         <v>37867.99999999999</v>
       </c>
       <c r="M25" t="n">
-        <v>1725327.064726412</v>
+        <v>397106.5589331404</v>
       </c>
       <c r="N25" t="n">
-        <v>25.90492510159179</v>
+        <v>0.9999999999999942</v>
       </c>
       <c r="O25" t="n">
         <v>2915.76176821649</v>
@@ -1800,7 +1800,7 @@
         <v>61373.67232632842</v>
       </c>
       <c r="L27" t="n">
-        <v>29602.9087374105</v>
+        <v>12579.47779916077</v>
       </c>
       <c r="M27" t="n">
         <v>3234408.767199999</v>
@@ -1809,10 +1809,10 @@
         <v>28.51419426482713</v>
       </c>
       <c r="O27" t="n">
-        <v>1635.642762831732</v>
+        <v>801.1041567238514</v>
       </c>
       <c r="P27" t="n">
-        <v>3002048.203665785</v>
+        <v>1155335.285561846</v>
       </c>
     </row>
     <row r="28">
@@ -1894,19 +1894,19 @@
         <v>194.9999999999991</v>
       </c>
       <c r="J29" t="n">
-        <v>497.8528815868382</v>
+        <v>257.8755753993303</v>
       </c>
       <c r="K29" t="n">
-        <v>61373.67232632842</v>
+        <v>2327.949027416018</v>
       </c>
       <c r="L29" t="n">
         <v>29602.9087374105</v>
       </c>
       <c r="M29" t="n">
-        <v>2185490.020395464</v>
+        <v>352889.0944825563</v>
       </c>
       <c r="N29" t="n">
-        <v>28.51419426482713</v>
+        <v>11.99999999999995</v>
       </c>
       <c r="O29" t="n">
         <v>3211</v>
@@ -1979,7 +1979,7 @@
         <v>69421.59999999999</v>
       </c>
       <c r="E31" t="n">
-        <v>692.2186286246737</v>
+        <v>104.0508328856842</v>
       </c>
       <c r="F31" t="n">
         <v>3389505.055700001</v>
@@ -1997,16 +1997,16 @@
         <v>497.8528815868382</v>
       </c>
       <c r="K31" t="n">
-        <v>61373.67232632842</v>
+        <v>19594.91258346423</v>
       </c>
       <c r="L31" t="n">
         <v>57789.99999999995</v>
       </c>
       <c r="M31" t="n">
-        <v>2185490.020395464</v>
+        <v>708166.2951166953</v>
       </c>
       <c r="N31" t="n">
-        <v>28.51419426482713</v>
+        <v>5.999999999999963</v>
       </c>
       <c r="O31" t="n">
         <v>3403</v>

</xml_diff>